<commit_message>
Steady state time is read from Scenarios.xlsx Fixes #323
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520BA030-A0B1-4F25-A2D6-A69FDBF709AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D972F274-E898-423E-9769-D64B5291C21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Indiv</t>
+  </si>
+  <si>
+    <t>SteadyStateTime</t>
+  </si>
+  <si>
+    <t>SteadyStateTimeUnit</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
@@ -409,25 +418,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="19.1328125" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -450,10 +459,16 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -475,11 +490,11 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -501,7 +516,13 @@
       <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>500</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -512,6 +533,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -748,17 +780,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -769,6 +790,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -787,17 +819,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add SteadyStateTime to ScenarioConfiguration (#364)
* Steady state time is read from Scenarios.xlsx
Fixes #323

* - Add `customFunction()` and `customFunctionArgs` to `ScenarioConfiguration`
- Add description of how to use `customFunction()` to the vignette
- Create dev version of docs

Fixes #319, #320, #348

* Typos in NEWS.md

* typos in standard workflow

Co-authored-by: Sergei Vavilov <svavil@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520BA030-A0B1-4F25-A2D6-A69FDBF709AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D972F274-E898-423E-9769-D64B5291C21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Indiv</t>
+  </si>
+  <si>
+    <t>SteadyStateTime</t>
+  </si>
+  <si>
+    <t>SteadyStateTimeUnit</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
@@ -409,25 +418,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="19.1328125" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -450,10 +459,16 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -475,11 +490,11 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -501,7 +516,13 @@
       <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>500</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -512,6 +533,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -748,17 +780,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -769,6 +790,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -787,17 +819,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Output paths are defined in the excel specification now.
Fixes #362
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65134C8F-2BD1-4EA5-AA25-C00EA765C847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A24F70-3132-47C6-8735-5EBAF15802C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
+    <sheet name="OutputPaths" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -101,6 +102,30 @@
   </si>
   <si>
     <t>TestPopulation</t>
+  </si>
+  <si>
+    <t>OutputPathsIds</t>
+  </si>
+  <si>
+    <t>OutputPathId</t>
+  </si>
+  <si>
+    <t>OutputPath</t>
+  </si>
+  <si>
+    <t>Aciclovir_PVB</t>
+  </si>
+  <si>
+    <t>Aciclovir_fat_cell</t>
+  </si>
+  <si>
+    <t>Organism|PeripheralVenousBlood|Aciclovir|Plasma (Peripheral Venous Blood)</t>
+  </si>
+  <si>
+    <t>Organism|Fat|Intracellular|Aciclovir|Concentration in container</t>
+  </si>
+  <si>
+    <t>Aciclovir_PVB, Aciclovir_fat_cell</t>
   </si>
 </sst>
 </file>
@@ -427,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,9 +469,10 @@
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -480,8 +506,11 @@
       <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -507,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -538,8 +567,11 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -574,18 +606,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA486CF-725F-421A-8D45-E3AE92A4A2C0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -822,7 +887,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -831,18 +896,18 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -861,10 +926,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Output paths in excel (#379)
* Clear WORDLIST as we dont have a spell check yet. Will have to populate the list anew.

* Output paths are defined in the excel specification now.

Fixes #362

* Typo in news
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65134C8F-2BD1-4EA5-AA25-C00EA765C847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A24F70-3132-47C6-8735-5EBAF15802C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
+    <sheet name="OutputPaths" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -101,6 +102,30 @@
   </si>
   <si>
     <t>TestPopulation</t>
+  </si>
+  <si>
+    <t>OutputPathsIds</t>
+  </si>
+  <si>
+    <t>OutputPathId</t>
+  </si>
+  <si>
+    <t>OutputPath</t>
+  </si>
+  <si>
+    <t>Aciclovir_PVB</t>
+  </si>
+  <si>
+    <t>Aciclovir_fat_cell</t>
+  </si>
+  <si>
+    <t>Organism|PeripheralVenousBlood|Aciclovir|Plasma (Peripheral Venous Blood)</t>
+  </si>
+  <si>
+    <t>Organism|Fat|Intracellular|Aciclovir|Concentration in container</t>
+  </si>
+  <si>
+    <t>Aciclovir_PVB, Aciclovir_fat_cell</t>
   </si>
 </sst>
 </file>
@@ -427,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,9 +469,10 @@
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -480,8 +506,11 @@
       <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -507,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -538,8 +567,11 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -574,18 +606,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA486CF-725F-421A-8D45-E3AE92A4A2C0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -822,7 +887,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -831,18 +896,18 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -861,10 +926,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- `runScenarios()` also returns a `Population` object for population simulations. - `runScenarios()` gets a new argument `savePopulationToCSV`, with default value `FALSE`. - `ScenarioConfiguration` gets a new field `readPopulationFromCSV`. If `FALSE` (default), a new population is created from defined population demographics. If `TRUE`, a simulation will be imported from a csv sheet located in the folder `Parameters/Populations` and named as the `PopulationId`.
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A24F70-3132-47C6-8735-5EBAF15802C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AFAC09-E7FF-41E5-8569-ACE7693E3B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Aciclovir_PVB, Aciclovir_fat_cell</t>
+  </si>
+  <si>
+    <t>ReadPopulationFromCSV</t>
+  </si>
+  <si>
+    <t>PopulationScenarioFromCSV</t>
   </si>
 </sst>
 </file>
@@ -452,27 +458,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -483,95 +492,95 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="b">
+      <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>500</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -581,22 +590,57 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="b">
+      <c r="I4" t="b">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve handling of populations in population scenarios (#422)
* - `runScenarios()` also returns a `Population` object for population simulations.
- `runScenarios()` gets a new argument `savePopulationToCSV`, with default value `FALSE`.
- `ScenarioConfiguration` gets a new field `readPopulationFromCSV`. If `FALSE` (default),
a new population is created from defined population demographics. If `TRUE`, a simulation
will be imported from a csv sheet located in the folder `Parameters/Populations` and
named as the `PopulationId`.

* Update test snaps

* Add showtext and imports to "Imports" to fix issue with TLF snapshots
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A24F70-3132-47C6-8735-5EBAF15802C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AFAC09-E7FF-41E5-8569-ACE7693E3B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Aciclovir_PVB, Aciclovir_fat_cell</t>
+  </si>
+  <si>
+    <t>ReadPopulationFromCSV</t>
+  </si>
+  <si>
+    <t>PopulationScenarioFromCSV</t>
   </si>
 </sst>
 </file>
@@ -452,27 +458,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -483,95 +492,95 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="b">
+      <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>500</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -581,22 +590,57 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="b">
+      <c r="I4" t="b">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Definition of simulation time in the `Scenarios.xlsx` file changed. The new expected format is a triplet of values <StartTime, EndTime, Resolution>, where `Resolution` is the number of simulated points per time unit defined in the column `TimeUnit`. - Field `poinstPerMinute` of `ScenarioConfiguration` has been removed.
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AFAC09-E7FF-41E5-8569-ACE7693E3B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDDAD20-A459-4B82-8D57-21D53FFF046A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -35,8 +35,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Pavel Balazki</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{1306E5C1-FB75-42DA-BC10-4285E9FAEE6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pavel Balazki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Simulation time is defined as time intervals.
+Expected is a triple of values {start, end, resolution}, resolution given in "points per &lt;time unit&gt;" as defined in the columne "SimulationTimeUnit". Multiple intervals can be separated by a ";"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -132,13 +167,22 @@
   </si>
   <si>
     <t>PopulationScenarioFromCSV</t>
+  </si>
+  <si>
+    <t>0, 24, 60</t>
+  </si>
+  <si>
+    <t>0, 1, 60; 1, 12, 20</t>
+  </si>
+  <si>
+    <t>0, 12, 20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +197,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -457,31 +514,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5859375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.87890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5859375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -522,7 +579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -535,8 +592,8 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>24</v>
+      <c r="G2" t="s">
+        <v>32</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -545,7 +602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -558,8 +615,8 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
-        <v>12</v>
+      <c r="G3" t="s">
+        <v>33</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -580,7 +637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -599,8 +656,8 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>12</v>
+      <c r="G4" t="s">
+        <v>34</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -612,7 +669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -631,8 +688,8 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
-        <v>12</v>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
@@ -647,6 +704,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -658,13 +716,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -672,7 +730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -680,7 +738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -695,6 +753,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -931,27 +1009,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -968,23 +1045,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Refine specification of output intervals in ScenarioConfiguration (#442)
* - Definition of simulation time in the `Scenarios.xlsx` file changed. The new expected format
is a triplet of values <StartTime, EndTime, Resolution>, where `Resolution` is the number of
simulated points per time unit defined in the column `TimeUnit`.
- Field `poinstPerMinute` of `ScenarioConfiguration` has been removed.

* Restore changes lost while merging develop
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Scenarios.xlsx
+++ b/tests/data/TestProject/Parameters/Scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AFAC09-E7FF-41E5-8569-ACE7693E3B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDDAD20-A459-4B82-8D57-21D53FFF046A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16973" yWindow="-93" windowWidth="25787" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -35,8 +35,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Pavel Balazki</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{1306E5C1-FB75-42DA-BC10-4285E9FAEE6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pavel Balazki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Simulation time is defined as time intervals.
+Expected is a triple of values {start, end, resolution}, resolution given in "points per &lt;time unit&gt;" as defined in the columne "SimulationTimeUnit". Multiple intervals can be separated by a ";"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -132,13 +167,22 @@
   </si>
   <si>
     <t>PopulationScenarioFromCSV</t>
+  </si>
+  <si>
+    <t>0, 24, 60</t>
+  </si>
+  <si>
+    <t>0, 1, 60; 1, 12, 20</t>
+  </si>
+  <si>
+    <t>0, 12, 20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +197,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -457,31 +514,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A1BACA-04A5-4461-B34D-CB73BA82CEC5}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5859375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.87890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5859375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -522,7 +579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -535,8 +592,8 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>24</v>
+      <c r="G2" t="s">
+        <v>32</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -545,7 +602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -558,8 +615,8 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
-        <v>12</v>
+      <c r="G3" t="s">
+        <v>33</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -580,7 +637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -599,8 +656,8 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>12</v>
+      <c r="G4" t="s">
+        <v>34</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -612,7 +669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -631,8 +688,8 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
-        <v>12</v>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
@@ -647,6 +704,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -658,13 +716,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -672,7 +730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -680,7 +738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -695,6 +753,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -931,27 +1009,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -968,23 +1045,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>